<commit_message>
feat: get data water quality
</commit_message>
<xml_diff>
--- a/app/data/dataset_limbah_cair_industri.xlsx
+++ b/app/data/dataset_limbah_cair_industri.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Drive\PNC\Penelitian\2024\DIPA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Learning\Magang\industrial-wastewater-quality-prediction\app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BAA755-055B-4C8A-8000-4BA912C2B3C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1176DE1-0E7C-4875-9CEF-EF20D2DF6BA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -418,7 +418,7 @@
   <dimension ref="A1:H366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>